<commit_message>
new meta types, filtered types for sample forms
</commit_message>
<xml_diff>
--- a/sarrive.xlsx
+++ b/sarrive.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>type</t>
   </si>
@@ -90,7 +90,7 @@
     <t>Scan Type</t>
   </si>
   <si>
-    <t>quick search('stypes')</t>
+    <t>quick search('stypes', 'contains', 'relevant', 'sarrive')</t>
   </si>
   <si>
     <t>select_one condition</t>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
   <si>
     <t>2. Sample Delivery</t>
@@ -608,7 +611,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.71"/>
+    <col customWidth="1" min="1" max="1" width="16.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -618,13 +621,19 @@
       <c r="B1" s="14" t="s">
         <v>49</v>
       </c>
+      <c r="C1" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2.016033001E9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>